<commit_message>
boy, I sure love cleaning
</commit_message>
<xml_diff>
--- a/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
+++ b/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Tiles</t>
   </si>
@@ -132,6 +132,42 @@
   </si>
   <si>
     <t>Is an NPC.</t>
+  </si>
+  <si>
+    <t>Map Construction</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Start X Position</t>
+  </si>
+  <si>
+    <t>Start Y Position</t>
+  </si>
+  <si>
+    <t>NPC Count</t>
+  </si>
+  <si>
+    <t>Map data</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Name (alpha-numeric)</t>
   </si>
 </sst>
 </file>
@@ -489,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,9 +542,11 @@
     <col min="9" max="9" width="9.140625" style="2"/>
     <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,11 +556,14 @@
       <c r="K1" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -553,8 +594,17 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -585,8 +635,17 @@
       <c r="L4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -617,8 +676,17 @@
       <c r="L5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -637,8 +705,17 @@
       <c r="L6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -657,8 +734,17 @@
       <c r="L7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -671,8 +757,17 @@
       <c r="D8" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -684,6 +779,27 @@
       </c>
       <c r="D9" s="2">
         <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>42</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <f>(50*50)-1</f>
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Yet another map extension
</commit_message>
<xml_diff>
--- a/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
+++ b/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Tiles</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Ascii 177</t>
   </si>
   <si>
-    <t>Colour.DARK_GREY</t>
-  </si>
-  <si>
     <t>Char</t>
   </si>
   <si>
@@ -56,18 +53,12 @@
     <t>Grass</t>
   </si>
   <si>
-    <t>Colour.GREEN</t>
-  </si>
-  <si>
     <t>w</t>
   </si>
   <si>
     <t>Water</t>
   </si>
   <si>
-    <t>Colour.BLUE</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -83,9 +74,6 @@
     <t>Brick/Wall</t>
   </si>
   <si>
-    <t>Colour.RED</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -128,9 +116,6 @@
     <t>Nothing can pass.</t>
   </si>
   <si>
-    <t>Sheep can't pass.</t>
-  </si>
-  <si>
     <t>Is an NPC.</t>
   </si>
   <si>
@@ -168,6 +153,48 @@
   </si>
   <si>
     <t>Name (alpha-numeric)</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>Pathway</t>
+  </si>
+  <si>
+    <t>Colour.GREY_40</t>
+  </si>
+  <si>
+    <t>Colour.GREEN_BB</t>
+  </si>
+  <si>
+    <t>Colour.BLUE_BB</t>
+  </si>
+  <si>
+    <t>Colour.RED_BB</t>
+  </si>
+  <si>
+    <t>Colour.GREY_70</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>Colour.GREY_D0</t>
+  </si>
+  <si>
+    <t>Sheep/Cow can't pass.</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Cow</t>
+  </si>
+  <si>
+    <t>Colour.BLACK</t>
   </si>
 </sst>
 </file>
@@ -525,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +568,7 @@
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="2"/>
     <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="9.140625" style="2"/>
   </cols>
@@ -551,13 +578,13 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -565,7 +592,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -577,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
@@ -589,42 +616,42 @@
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I4" s="2">
         <v>3</v>
@@ -633,16 +660,16 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -653,19 +680,19 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I5" s="2">
         <v>3</v>
@@ -674,56 +701,68 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
         <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>38</v>
       </c>
       <c r="O5" s="2">
         <v>1</v>
       </c>
       <c r="P5" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
       <c r="K6" s="2">
         <v>2</v>
       </c>
       <c r="L6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" t="s">
         <v>34</v>
-      </c>
-      <c r="N6" t="s">
-        <v>39</v>
       </c>
       <c r="O6" s="2">
         <v>1</v>
       </c>
       <c r="P6" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -732,74 +771,100 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
         <v>35</v>
-      </c>
-      <c r="N7" t="s">
-        <v>40</v>
       </c>
       <c r="O7" s="2">
         <v>0</v>
       </c>
       <c r="P7" s="2">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
       </c>
       <c r="N8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="O8" s="2">
         <v>0</v>
       </c>
       <c r="P8" s="2">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O9" s="2">
         <v>0</v>
       </c>
       <c r="P9" s="2">
-        <f>(50*50)-1</f>
-        <v>2499</v>
+        <f>(60*60)-1</f>
+        <v>3599</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
       <c r="N10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>44</v>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i'm beginning to feel like a refactgod
</commit_message>
<xml_diff>
--- a/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
+++ b/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>Tiles</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Water</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>Bank</t>
   </si>
   <si>
@@ -195,6 +192,30 @@
   </si>
   <si>
     <t>Colour.BLACK</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Wall</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>Entrance</t>
+  </si>
+  <si>
+    <t>TBC</t>
   </si>
 </sst>
 </file>
@@ -552,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,13 +599,13 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -616,42 +637,42 @@
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2">
         <v>3</v>
@@ -660,16 +681,16 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -680,19 +701,19 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
         <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
       </c>
       <c r="I5" s="2">
         <v>3</v>
@@ -701,10 +722,10 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O5" s="2">
         <v>1</v>
@@ -721,19 +742,19 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>56</v>
       </c>
       <c r="I6" s="2">
         <v>3</v>
@@ -742,10 +763,10 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O6" s="2">
         <v>1</v>
@@ -762,7 +783,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -771,10 +792,10 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="2">
         <v>0</v>
@@ -785,19 +806,19 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
       </c>
       <c r="N8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O8" s="2">
         <v>0</v>
@@ -808,19 +829,19 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O9" s="2">
         <v>0</v>
@@ -832,38 +853,80 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
       <c r="N10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="P10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
       <c r="D11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
saving to appdata, objects are no fun (0.8.1)
</commit_message>
<xml_diff>
--- a/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
+++ b/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>Tiles</t>
   </si>
@@ -140,18 +140,12 @@
     <t>Map data</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
     <t>Max</t>
   </si>
   <si>
-    <t>Name (alpha-numeric)</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -216,14 +210,65 @@
   </si>
   <si>
     <t>TBC</t>
+  </si>
+  <si>
+    <t>Name (AlphaNumeric)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Extra map count</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note: See example below on how the document </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MUST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> be formatted.</t>
+    </r>
+  </si>
+  <si>
+    <t>*'null' is acceptable as it appears here, without the quotes if you don't wish there to be a map in that direction.</t>
+  </si>
+  <si>
+    <t>Note: You must include a map for each of the four directions.* Left, up, right and down, in that order and include extra maps if any under that.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -274,6 +319,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24FFF7C1-7258-4CBC-8481-A749AF1CB716}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="21239" t="12647" r="46143" b="33553"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9401175" y="2657475"/>
+          <a:ext cx="2752725" cy="2552700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -573,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,10 +739,10 @@
         <v>31</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -684,13 +777,13 @@
         <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>38</v>
+        <v>62</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -701,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -742,19 +835,19 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" t="s">
         <v>53</v>
-      </c>
-      <c r="G6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" t="s">
-        <v>55</v>
       </c>
       <c r="I6" s="2">
         <v>3</v>
@@ -763,7 +856,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N6" t="s">
         <v>33</v>
@@ -783,7 +876,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -806,7 +899,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -835,7 +928,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -853,50 +946,59 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>37</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>38</v>
+        <v>64</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
+      <c r="P11" s="2">
+        <v>3600</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -904,33 +1006,48 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s">
-        <v>63</v>
-      </c>
       <c r="D13" s="2">
         <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inside buildings (Mary Poppins)
</commit_message>
<xml_diff>
--- a/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
+++ b/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>Tiles</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>Note: You must include a map for each of the four directions.* Left, up, right and down, in that order and include extra maps if any under that.</t>
+  </si>
+  <si>
+    <t>Map Doors</t>
+  </si>
+  <si>
+    <t>Is a door.</t>
   </si>
 </sst>
 </file>
@@ -325,16 +331,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -356,7 +362,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9401175" y="2657475"/>
+          <a:off x="9420225" y="2857500"/>
           <a:ext cx="2752725" cy="2552700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -669,7 +675,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +774,7 @@
         <v>17</v>
       </c>
       <c r="I4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
@@ -809,7 +815,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" s="2">
         <v>1</v>
@@ -850,7 +856,7 @@
         <v>53</v>
       </c>
       <c r="I6" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6" s="2">
         <v>2</v>
@@ -885,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="N7" t="s">
         <v>34</v>
@@ -910,6 +916,12 @@
       <c r="D8" s="2">
         <v>2</v>
       </c>
+      <c r="K8" s="2">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
       <c r="N8" t="s">
         <v>35</v>
       </c>
@@ -981,10 +993,10 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="O11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="2">
         <v>3600</v>
@@ -1003,6 +1015,15 @@
       <c r="D12" s="2">
         <v>1</v>
       </c>
+      <c r="N12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
+      <c r="P12" s="2">
+        <v>3600</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1017,9 +1038,6 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="N13" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1032,7 +1050,10 @@
         <v>61</v>
       </c>
       <c r="D14" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="14:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed weird saving bug
</commit_message>
<xml_diff>
--- a/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
+++ b/out/production/JAVA-RhythmMachine/documentation/tiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Tiles</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Is a door.</t>
+  </si>
+  <si>
+    <t>Map Flags</t>
   </si>
 </sst>
 </file>
@@ -332,15 +335,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -362,7 +365,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9420225" y="2857500"/>
+          <a:off x="9410700" y="3038475"/>
           <a:ext cx="2752725" cy="2552700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -674,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,14 +949,13 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2">
-        <f>(60*60)-1</f>
-        <v>3599</v>
+        <v>1</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -970,13 +972,14 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="O10" s="2">
         <v>0</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>63</v>
+      <c r="P10" s="2">
+        <f>(60*60)-1</f>
+        <v>3599</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -993,13 +996,13 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="O11" s="2">
         <v>0</v>
       </c>
-      <c r="P11" s="2">
-        <v>3600</v>
+      <c r="P11" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1016,10 +1019,10 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="O12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" s="2">
         <v>3600</v>
@@ -1038,6 +1041,15 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
+      <c r="N13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
+      <c r="P13" s="2">
+        <v>3600</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1052,7 +1064,9 @@
       <c r="D14" s="2">
         <v>3</v>
       </c>
-      <c r="N14" t="s">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>